<commit_message>
add some verification of Zhishang inheritance work
</commit_message>
<xml_diff>
--- a/Project_Inheritance_Documentation/Branch_1_Inheritance/Zhishang_Bian_Inheritance.xlsx
+++ b/Project_Inheritance_Documentation/Branch_1_Inheritance/Zhishang_Bian_Inheritance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f337a85aa8871bf9/Desktop/japanese_project/japanese-handwriting-analysis/Project_Inheritance_Documentation/Branch_1_Inheritance/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANU\Semester_3\Advanced_Computing_Project\Project_Repo\japanese-handwriting-analysis\Project_Inheritance_Documentation\Branch_1_Inheritance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{19693DD5-738C-42A8-9A5B-841EA747F7C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F251761F-BA76-472D-BA93-D3A7297358F8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198DF6E0-3D73-4EC3-9FFD-3D889A3FA9C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="90">
   <si>
     <t>How to Use It</t>
   </si>
@@ -360,6 +358,15 @@
   </si>
   <si>
     <t xml:space="preserve"> Issues </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes, we are completely aware of this word segmentation task and risk associated with it </t>
+  </si>
+  <si>
+    <t>Zhishang told us regarding this and about the API that was going to be expired</t>
+  </si>
+  <si>
+    <t>Next semester, we continuing members will have to figure out how bring up some alternative for the expired software</t>
   </si>
 </sst>
 </file>
@@ -432,7 +439,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -492,12 +499,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -535,6 +553,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -818,28 +839,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O39"/>
+  <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="95" zoomScaleNormal="78" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="95" zoomScaleNormal="78" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K6" sqref="K6"/>
+      <selection pane="bottomLeft" activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="17.1328125" customWidth="1"/>
-    <col min="5" max="5" width="50.46484375" customWidth="1"/>
-    <col min="6" max="6" width="41.53125" customWidth="1"/>
-    <col min="7" max="7" width="21.19921875" customWidth="1"/>
-    <col min="8" max="8" width="40.19921875" customWidth="1"/>
-    <col min="9" max="11" width="21.46484375" customWidth="1"/>
-    <col min="12" max="12" width="42.46484375" customWidth="1"/>
-    <col min="13" max="14" width="21.46484375" customWidth="1"/>
+    <col min="1" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="50.42578125" customWidth="1"/>
+    <col min="6" max="6" width="41.5703125" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" customWidth="1"/>
+    <col min="8" max="8" width="40.140625" customWidth="1"/>
+    <col min="9" max="11" width="21.42578125" customWidth="1"/>
+    <col min="12" max="12" width="42.42578125" customWidth="1"/>
+    <col min="13" max="13" width="24" customWidth="1"/>
+    <col min="14" max="14" width="21.42578125" customWidth="1"/>
     <col min="15" max="15" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="A1" s="9" t="s">
         <v>18</v>
       </c>
@@ -860,7 +882,7 @@
       <c r="N1" s="13"/>
       <c r="O1" s="14"/>
     </row>
-    <row r="2" spans="1:15" ht="28.5">
+    <row r="2" spans="1:16" ht="30">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -907,7 +929,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="42.75">
+    <row r="3" spans="1:16" ht="45">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
@@ -938,7 +960,7 @@
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
     </row>
-    <row r="4" spans="1:15" ht="54" customHeight="1">
+    <row r="4" spans="1:16" ht="54" customHeight="1">
       <c r="A4" s="5">
         <v>1</v>
       </c>
@@ -975,11 +997,17 @@
       <c r="L4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-    </row>
-    <row r="5" spans="1:15" ht="54" customHeight="1">
+      <c r="M4" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="O4" s="15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="54" customHeight="1">
       <c r="A5" s="5">
         <v>2</v>
       </c>
@@ -1019,8 +1047,9 @@
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
-    </row>
-    <row r="6" spans="1:15" ht="54" customHeight="1">
+      <c r="P5" s="5"/>
+    </row>
+    <row r="6" spans="1:16" ht="54" customHeight="1">
       <c r="A6" s="5">
         <v>3</v>
       </c>
@@ -1061,7 +1090,7 @@
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
     </row>
-    <row r="7" spans="1:15" ht="54" customHeight="1">
+    <row r="7" spans="1:16" ht="54" customHeight="1">
       <c r="A7" s="5">
         <v>4</v>
       </c>
@@ -1102,7 +1131,7 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
     </row>
-    <row r="8" spans="1:15" ht="54" customHeight="1">
+    <row r="8" spans="1:16" ht="54" customHeight="1">
       <c r="A8" s="5">
         <v>5</v>
       </c>
@@ -1143,7 +1172,7 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
     </row>
-    <row r="9" spans="1:15" ht="109.25" customHeight="1">
+    <row r="9" spans="1:16" ht="109.35" customHeight="1">
       <c r="A9" s="5">
         <v>6</v>
       </c>
@@ -1184,7 +1213,7 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
     </row>
-    <row r="10" spans="1:15" ht="54" customHeight="1">
+    <row r="10" spans="1:16" ht="54" customHeight="1">
       <c r="A10" s="5">
         <v>7</v>
       </c>
@@ -1225,7 +1254,7 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
     </row>
-    <row r="11" spans="1:15" ht="54" customHeight="1">
+    <row r="11" spans="1:16" ht="54" customHeight="1">
       <c r="A11" s="5">
         <v>8</v>
       </c>
@@ -1266,7 +1295,7 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" spans="1:15" ht="65.45" customHeight="1">
+    <row r="12" spans="1:16" ht="65.45" customHeight="1">
       <c r="A12" s="5">
         <v>9</v>
       </c>
@@ -1307,7 +1336,7 @@
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" spans="1:15" ht="88.25" customHeight="1">
+    <row r="13" spans="1:16" ht="88.35" customHeight="1">
       <c r="A13" s="5">
         <v>10</v>
       </c>
@@ -1348,7 +1377,7 @@
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" spans="1:15" ht="54" customHeight="1">
+    <row r="14" spans="1:16" ht="54" customHeight="1">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -1365,7 +1394,7 @@
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
     </row>
-    <row r="15" spans="1:15" ht="54" customHeight="1">
+    <row r="15" spans="1:16" ht="54" customHeight="1">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -1382,7 +1411,7 @@
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
     </row>
-    <row r="16" spans="1:15" ht="54" customHeight="1">
+    <row r="16" spans="1:16" ht="54" customHeight="1">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>

</xml_diff>

<commit_message>
Complete verification of Zhishang work inheritance
</commit_message>
<xml_diff>
--- a/Project_Inheritance_Documentation/Branch_1_Inheritance/Zhishang_Bian_Inheritance.xlsx
+++ b/Project_Inheritance_Documentation/Branch_1_Inheritance/Zhishang_Bian_Inheritance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANU\Semester_3\Advanced_Computing_Project\Project_Repo\japanese-handwriting-analysis\Project_Inheritance_Documentation\Branch_1_Inheritance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198DF6E0-3D73-4EC3-9FFD-3D889A3FA9C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62543BCF-D900-4C7E-891C-20E7599EDBF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="116">
   <si>
     <t>How to Use It</t>
   </si>
@@ -367,6 +367,84 @@
   </si>
   <si>
     <t>Next semester, we continuing members will have to figure out how bring up some alternative for the expired software</t>
+  </si>
+  <si>
+    <t>Yes, we ran this on my(Arslan's) laptop and it worked completely fine</t>
+  </si>
+  <si>
+    <t>Understood the Japanese and Chinese OCR and it worked completely fine on my system</t>
+  </si>
+  <si>
+    <t>Next Semester, I can explain this thing to new members and also work myself on this</t>
+  </si>
+  <si>
+    <t>Yes, understood what this task meant</t>
+  </si>
+  <si>
+    <t>Can do it myself or assign to someone else from group member to do this.</t>
+  </si>
+  <si>
+    <t>This part is easy to manage, so can comfortably do in next semester</t>
+  </si>
+  <si>
+    <t>Yes, understood this one from Zhishang</t>
+  </si>
+  <si>
+    <t>It runs on my(Arslan's) laptop and this part is already finished</t>
+  </si>
+  <si>
+    <t>Can explain it to the members in next semester that what this task was all about and what we achieved in this.</t>
+  </si>
+  <si>
+    <t>Yes, understood this one from Zhishang and can continue on improving it next semester</t>
+  </si>
+  <si>
+    <t>It runs on my(Arslan's) laptop and this part is already finished but need some tests according to Dr Muhammad guidance/suggestion and we can do it in the next semester</t>
+  </si>
+  <si>
+    <t>Understood this task and can explain and assign it to new members next semester as well.</t>
+  </si>
+  <si>
+    <t>Yes, Zhishang told me regarding this issue and we will need to find a way/solution to solve this out</t>
+  </si>
+  <si>
+    <t>This is actually a risk that remains unresolved and will need to figure out it in next semester</t>
+  </si>
+  <si>
+    <t>I know some background of this issue as explained to me by Zhishang and can work on this in next semester with the new members</t>
+  </si>
+  <si>
+    <t>Yes, Zhishang explained me regarding this</t>
+  </si>
+  <si>
+    <t>I know regarding the image preprocessing and this part specifically,so can work on this thing and can also assign it to new members as well.</t>
+  </si>
+  <si>
+    <t>It runs on my laptop, but image preprocessing remained unfinished so that's why it couldn't get completed this time, so will have to finish image processing part first and then can continue on this thing.</t>
+  </si>
+  <si>
+    <t>Yes, Zhishang told me that Branch 1 isn't merged with Branch 2 yet.</t>
+  </si>
+  <si>
+    <t>Right now, I don’t have any comprehensive understanding of Branch 1 &amp; Branch 2, but will try to study these branches over the holiday period and will try to initiate this part as well.</t>
+  </si>
+  <si>
+    <t>This part will require a good understanding of both the branches and both time and effort as well.</t>
+  </si>
+  <si>
+    <t>Yes, understood this task</t>
+  </si>
+  <si>
+    <t>It runs on my laptop, and it's kind of almost completed but still requires some more improvement.</t>
+  </si>
+  <si>
+    <t>This is not a high priority task but can complete it after all the vital tasks are finished.</t>
+  </si>
+  <si>
+    <t>Yes, understood this task from Zhishang</t>
+  </si>
+  <si>
+    <t>Can explain it to the members in next semester that what this task is and what we need to improve on this and how.</t>
   </si>
 </sst>
 </file>
@@ -537,6 +615,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -553,9 +634,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -841,9 +919,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="95" zoomScaleNormal="78" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="78" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M6" sqref="M6"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -856,31 +934,31 @@
     <col min="8" max="8" width="40.140625" customWidth="1"/>
     <col min="9" max="11" width="21.42578125" customWidth="1"/>
     <col min="12" max="12" width="42.42578125" customWidth="1"/>
-    <col min="13" max="13" width="24" customWidth="1"/>
-    <col min="14" max="14" width="21.42578125" customWidth="1"/>
-    <col min="15" max="15" width="23" customWidth="1"/>
+    <col min="13" max="13" width="28.7109375" customWidth="1"/>
+    <col min="14" max="14" width="44.7109375" customWidth="1"/>
+    <col min="15" max="15" width="34.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="12" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="13"/>
-      <c r="O1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="15"/>
     </row>
     <row r="2" spans="1:16" ht="30">
       <c r="A2" s="2" t="s">
@@ -1003,7 +1081,7 @@
       <c r="N4" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="O4" s="15" t="s">
+      <c r="O4" s="9" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1044,9 +1122,15 @@
       <c r="L5" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
+      <c r="M5" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>92</v>
+      </c>
       <c r="P5" s="5"/>
     </row>
     <row r="6" spans="1:16" ht="54" customHeight="1">
@@ -1086,9 +1170,15 @@
       <c r="L6" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
+      <c r="M6" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="7" spans="1:16" ht="54" customHeight="1">
       <c r="A7" s="5">
@@ -1127,9 +1217,15 @@
       <c r="L7" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
+      <c r="M7" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="8" spans="1:16" ht="54" customHeight="1">
       <c r="A8" s="5">
@@ -1168,9 +1264,15 @@
       <c r="L8" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
+      <c r="M8" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="9" spans="1:16" ht="109.35" customHeight="1">
       <c r="A9" s="5">
@@ -1209,9 +1311,15 @@
       <c r="L9" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
+      <c r="M9" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="O9" s="5" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="10" spans="1:16" ht="54" customHeight="1">
       <c r="A10" s="5">
@@ -1250,9 +1358,15 @@
       <c r="L10" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
+      <c r="M10" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="11" spans="1:16" ht="54" customHeight="1">
       <c r="A11" s="5">
@@ -1291,9 +1405,15 @@
       <c r="L11" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
+      <c r="M11" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="12" spans="1:16" ht="65.45" customHeight="1">
       <c r="A12" s="5">
@@ -1332,9 +1452,15 @@
       <c r="L12" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
+      <c r="M12" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="O12" s="5" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="13" spans="1:16" ht="88.35" customHeight="1">
       <c r="A13" s="5">
@@ -1373,9 +1499,15 @@
       <c r="L13" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
+      <c r="M13" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="N13" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="O13" s="5" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="14" spans="1:16" ht="54" customHeight="1">
       <c r="A14" s="5"/>

</xml_diff>

<commit_message>
Edits and Mingbo's inheritance
</commit_message>
<xml_diff>
--- a/Project_Inheritance_Documentation/Branch_1_Inheritance/Zhishang_Bian_Inheritance.xlsx
+++ b/Project_Inheritance_Documentation/Branch_1_Inheritance/Zhishang_Bian_Inheritance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANU\Semester_3\Advanced_Computing_Project\Project_Repo\japanese-handwriting-analysis\Project_Inheritance_Documentation\Branch_1_Inheritance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f337a85aa8871bf9/Desktop/japanese_project/japanese-handwriting-analysis/Project_Inheritance_Documentation/Branch_1_Inheritance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62543BCF-D900-4C7E-891C-20E7599EDBF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{62543BCF-D900-4C7E-891C-20E7599EDBF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37DE1FD7-36C0-4B5D-B453-ADFFE3D1D218}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="115">
   <si>
     <t>How to Use It</t>
   </si>
@@ -57,9 +57,6 @@
     <t>List missing pieces (code, documentation, resources, etc.) that need to be transferred or clarified.</t>
   </si>
   <si>
-    <t>Name of the person inheriting the task.</t>
-  </si>
-  <si>
     <t>Date by which handover needs to be completed.</t>
   </si>
   <si>
@@ -172,10 +169,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Arslan</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Already finished</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -201,10 +194,6 @@
   </si>
   <si>
     <t>Need docstring</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Student in next semester who are responsible for branch1</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -445,6 +434,12 @@
   </si>
   <si>
     <t>Can explain it to the members in next semester that what this task is and what we need to improve on this and how.</t>
+  </si>
+  <si>
+    <t>Name of the person passing the inheritance.</t>
+  </si>
+  <si>
+    <t>Zhishang</t>
   </si>
 </sst>
 </file>
@@ -615,7 +610,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -919,29 +914,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="78" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="95" zoomScaleNormal="78" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="17.140625" customWidth="1"/>
-    <col min="5" max="5" width="50.42578125" customWidth="1"/>
-    <col min="6" max="6" width="41.5703125" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" customWidth="1"/>
-    <col min="8" max="8" width="40.140625" customWidth="1"/>
-    <col min="9" max="11" width="21.42578125" customWidth="1"/>
-    <col min="12" max="12" width="42.42578125" customWidth="1"/>
-    <col min="13" max="13" width="28.7109375" customWidth="1"/>
-    <col min="14" max="14" width="44.7109375" customWidth="1"/>
-    <col min="15" max="15" width="34.85546875" customWidth="1"/>
+    <col min="1" max="2" width="6.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.1328125" customWidth="1"/>
+    <col min="5" max="5" width="50.3984375" customWidth="1"/>
+    <col min="6" max="6" width="41.59765625" customWidth="1"/>
+    <col min="7" max="7" width="21.1328125" customWidth="1"/>
+    <col min="8" max="8" width="40.1328125" customWidth="1"/>
+    <col min="9" max="11" width="21.3984375" customWidth="1"/>
+    <col min="12" max="12" width="42.3984375" customWidth="1"/>
+    <col min="13" max="13" width="28.73046875" customWidth="1"/>
+    <col min="14" max="14" width="44.73046875" customWidth="1"/>
+    <col min="15" max="15" width="34.86328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -955,63 +950,63 @@
       <c r="K1" s="11"/>
       <c r="L1" s="12"/>
       <c r="M1" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N1" s="14"/>
       <c r="O1" s="15"/>
     </row>
-    <row r="2" spans="1:16" ht="30">
+    <row r="2" spans="1:16" ht="28.5">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="N2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="45">
+    </row>
+    <row r="3" spans="1:16" ht="42.75">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
@@ -1027,10 +1022,10 @@
         <v>6</v>
       </c>
       <c r="I3" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -1043,46 +1038,46 @@
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="5" t="s">
+      <c r="F4" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="L4" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="K4" s="6" t="s">
+      <c r="M4" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="O4" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="O4" s="9" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="54" customHeight="1">
@@ -1093,43 +1088,43 @@
         <v>1</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="I5" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="J5" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="K5" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="L5" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="J5" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>42</v>
-      </c>
       <c r="M5" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="O5" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="P5" s="5"/>
     </row>
@@ -1141,43 +1136,43 @@
         <v>1</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="H6" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="I6" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="J6" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="K6" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="I6" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="L6" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="54" customHeight="1">
@@ -1188,43 +1183,43 @@
         <v>1</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="I7" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="J7" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="K7" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="L7" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="J7" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="L7" s="5" t="s">
-        <v>42</v>
-      </c>
       <c r="M7" s="5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="54" customHeight="1">
@@ -1235,43 +1230,43 @@
         <v>1</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="5" t="s">
+      <c r="G8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="I8" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="L8" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="G8" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="L8" s="5" t="s">
-        <v>62</v>
-      </c>
       <c r="M8" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="109.35" customHeight="1">
@@ -1282,43 +1277,43 @@
         <v>1</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E9" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="L9" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>66</v>
-      </c>
       <c r="M9" s="5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="O9" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="54" customHeight="1">
@@ -1329,43 +1324,43 @@
         <v>1</v>
       </c>
       <c r="C10" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="5" t="s">
+      <c r="G10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="L10" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="F10" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="L10" s="5" t="s">
-        <v>72</v>
-      </c>
       <c r="M10" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="O10" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="54" customHeight="1">
@@ -1373,46 +1368,46 @@
         <v>8</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>48</v>
+        <v>114</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="O11" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="65.45" customHeight="1">
@@ -1423,43 +1418,43 @@
         <v>1</v>
       </c>
       <c r="C12" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="5" t="s">
+      <c r="I12" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="J12" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="K12" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="G12" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H12" s="5" t="s">
+      <c r="L12" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="I12" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="K12" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="L12" s="5" t="s">
-        <v>82</v>
-      </c>
       <c r="M12" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="N12" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="O12" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="88.35" customHeight="1">
@@ -1470,43 +1465,43 @@
         <v>1</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F13" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="K13" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="G13" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="K13" s="8" t="s">
-        <v>81</v>
-      </c>
       <c r="L13" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="N13" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="O13" s="5" t="s">
         <v>112</v>
-      </c>
-      <c r="O13" s="5" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="54" customHeight="1">

</xml_diff>

<commit_message>
New Entries added for Branch 1 document
</commit_message>
<xml_diff>
--- a/Project_Inheritance_Documentation/Branch_1_Inheritance/Zhishang_Bian_Inheritance.xlsx
+++ b/Project_Inheritance_Documentation/Branch_1_Inheritance/Zhishang_Bian_Inheritance.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f337a85aa8871bf9/Desktop/japanese_project/japanese-handwriting-analysis/Project_Inheritance_Documentation/Branch_1_Inheritance/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jinpaiduizhang\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{62543BCF-D900-4C7E-891C-20E7599EDBF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37DE1FD7-36C0-4B5D-B453-ADFFE3D1D218}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3447C165-7748-4BCB-8CF9-1D10018AD22F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="122">
   <si>
     <t>How to Use It</t>
   </si>
@@ -440,17 +440,44 @@
   </si>
   <si>
     <t>Zhishang</t>
+  </si>
+  <si>
+    <t>There is a cell that require classify_pilot, it is from branch 2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>People who compile the code in "chi+jap_ocr" will be stopped because they need a classify csv to help OCR. That piece of code is from "Simple_cnn"</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Run "Simple_cnn" before run "chi+jap_ocr".</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Code not connected so that these might be a little bit complex</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zhishang</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Already finished but can need to be connected</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>OCR/Simple_cnn.py · main · Yuyang Han / Japanese Handwriting Analysis · GitLab (anu.edu.au)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -458,7 +485,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -466,13 +493,13 @@
       <b/>
       <sz val="11"/>
       <color theme="0" tint="-0.14999847407452621"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -481,7 +508,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -588,7 +615,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -631,10 +658,13 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -914,27 +944,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="95" zoomScaleNormal="78" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="95" zoomScaleNormal="78" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="6.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="17.1328125" customWidth="1"/>
-    <col min="5" max="5" width="50.3984375" customWidth="1"/>
-    <col min="6" max="6" width="41.59765625" customWidth="1"/>
-    <col min="7" max="7" width="21.1328125" customWidth="1"/>
-    <col min="8" max="8" width="40.1328125" customWidth="1"/>
-    <col min="9" max="11" width="21.3984375" customWidth="1"/>
-    <col min="12" max="12" width="42.3984375" customWidth="1"/>
-    <col min="13" max="13" width="28.73046875" customWidth="1"/>
-    <col min="14" max="14" width="44.73046875" customWidth="1"/>
-    <col min="15" max="15" width="34.86328125" customWidth="1"/>
+    <col min="1" max="2" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.109375" customWidth="1"/>
+    <col min="5" max="5" width="50.44140625" customWidth="1"/>
+    <col min="6" max="6" width="41.5546875" customWidth="1"/>
+    <col min="7" max="7" width="21.109375" customWidth="1"/>
+    <col min="8" max="8" width="40.109375" customWidth="1"/>
+    <col min="9" max="11" width="21.44140625" customWidth="1"/>
+    <col min="12" max="12" width="42.44140625" customWidth="1"/>
+    <col min="13" max="13" width="28.77734375" customWidth="1"/>
+    <col min="14" max="14" width="44.77734375" customWidth="1"/>
+    <col min="15" max="15" width="34.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>17</v>
       </c>
@@ -955,7 +985,7 @@
       <c r="N1" s="14"/>
       <c r="O1" s="15"/>
     </row>
-    <row r="2" spans="1:16" ht="28.5">
+    <row r="2" spans="1:16" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -1002,7 +1032,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="42.75">
+    <row r="3" spans="1:16" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
@@ -1033,7 +1063,7 @@
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
     </row>
-    <row r="4" spans="1:16" ht="54" customHeight="1">
+    <row r="4" spans="1:16" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>1</v>
       </c>
@@ -1080,7 +1110,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="54" customHeight="1">
+    <row r="5" spans="1:16" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>2</v>
       </c>
@@ -1128,7 +1158,7 @@
       </c>
       <c r="P5" s="5"/>
     </row>
-    <row r="6" spans="1:16" ht="54" customHeight="1">
+    <row r="6" spans="1:16" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>3</v>
       </c>
@@ -1175,7 +1205,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="54" customHeight="1">
+    <row r="7" spans="1:16" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>4</v>
       </c>
@@ -1222,7 +1252,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="54" customHeight="1">
+    <row r="8" spans="1:16" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>5</v>
       </c>
@@ -1269,7 +1299,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="109.35" customHeight="1">
+    <row r="9" spans="1:16" ht="109.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>6</v>
       </c>
@@ -1316,7 +1346,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="54" customHeight="1">
+    <row r="10" spans="1:16" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>7</v>
       </c>
@@ -1363,7 +1393,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="54" customHeight="1">
+    <row r="11" spans="1:16" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>8</v>
       </c>
@@ -1410,7 +1440,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="65.45" customHeight="1">
+    <row r="12" spans="1:16" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>9</v>
       </c>
@@ -1457,7 +1487,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="88.35" customHeight="1">
+    <row r="13" spans="1:16" ht="88.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>10</v>
       </c>
@@ -1504,24 +1534,54 @@
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="54" customHeight="1">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-    </row>
-    <row r="15" spans="1:16" ht="54" customHeight="1">
+    <row r="14" spans="1:16" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>11</v>
+      </c>
+      <c r="B14" s="5">
+        <v>1</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="K14" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="M14" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="N14" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="O14" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -1538,7 +1598,7 @@
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
     </row>
-    <row r="16" spans="1:16" ht="54" customHeight="1">
+    <row r="16" spans="1:16" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -1555,7 +1615,7 @@
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
     </row>
-    <row r="17" spans="1:15" ht="54" customHeight="1">
+    <row r="17" spans="1:15" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -1572,7 +1632,7 @@
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1589,7 +1649,7 @@
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1606,7 +1666,7 @@
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1623,7 +1683,7 @@
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1640,7 +1700,7 @@
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1657,7 +1717,7 @@
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1674,7 +1734,7 @@
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1691,7 +1751,7 @@
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1708,7 +1768,7 @@
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1725,7 +1785,7 @@
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1742,7 +1802,7 @@
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1759,7 +1819,7 @@
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1776,7 +1836,7 @@
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1793,7 +1853,7 @@
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1810,7 +1870,7 @@
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1827,7 +1887,7 @@
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1844,7 +1904,7 @@
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1861,7 +1921,7 @@
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1878,7 +1938,7 @@
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1895,7 +1955,7 @@
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1912,7 +1972,7 @@
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1929,7 +1989,7 @@
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1962,8 +2022,9 @@
     <hyperlink ref="K10" r:id="rId7" display="https://gitlab.cecs.anu.edu.au/u7434576/japanese-handwriting-analysis/-/issues/74" xr:uid="{233771A2-4DD2-4DF8-9416-000D4463E9A4}"/>
     <hyperlink ref="K12" r:id="rId8" xr:uid="{81C8DFCF-19F1-433D-A6C8-17833EE4D45E}"/>
     <hyperlink ref="K13" r:id="rId9" xr:uid="{39EE02EF-D98B-43D0-8707-144EA7841526}"/>
+    <hyperlink ref="K14" r:id="rId10" display="https://gitlab.cecs.anu.edu.au/u7434576/japanese-handwriting-analysis/-/blob/main/OCR/Simple_cnn.py?ref_type=heads" xr:uid="{72D30472-4A8C-456E-B0CC-298861A564AE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>